<commit_message>
Alterações no upload e botões
</commit_message>
<xml_diff>
--- a/ProjetoMFMovelaria/ProjetoMFMovelaria/ExcelFile/teste.xlsx
+++ b/ProjetoMFMovelaria/ProjetoMFMovelaria/ExcelFile/teste.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Email</t>
   </si>
@@ -36,13 +36,16 @@
     <t>Preço</t>
   </si>
   <si>
-    <t>Chaoa MDF 18mm Branco</t>
-  </si>
-  <si>
     <t>MDF</t>
   </si>
   <si>
-    <t>leandro@hotmail.com</t>
+    <t>Tabata</t>
+  </si>
+  <si>
+    <t>Batata</t>
+  </si>
+  <si>
+    <t>batateira@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -116,13 +119,11 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="thin">
         <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
+      </left>
+      <right/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -134,27 +135,21 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -162,9 +157,139 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F3" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A1:F3"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Email"/>
+    <tableColumn id="2" name="Total do orçamento"/>
+    <tableColumn id="3" name="Desrição" dataDxfId="3"/>
+    <tableColumn id="4" name="Tipo" dataDxfId="2"/>
+    <tableColumn id="5" name="Quantidade" dataDxfId="1"/>
+    <tableColumn id="6" name="Preço" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -452,7 +577,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -461,7 +586,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="33.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
@@ -469,43 +594,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1">
+        <v>554</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4">
-        <v>454</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2</v>
-      </c>
-      <c r="F2" s="6">
-        <v>227</v>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -514,6 +655,9 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>